<commit_message>
-Reinitialisation de la donnée est préparation migration des donnees
</commit_message>
<xml_diff>
--- a/Conception/PCG.xlsx
+++ b/Conception/PCG.xlsx
@@ -1375,8 +1375,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B318"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A297" workbookViewId="0">
-      <selection activeCell="C306" sqref="C306"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>